<commit_message>
Versionsübersicht v1.2.0 dbApplication, v1.6.0 dbJournal
</commit_message>
<xml_diff>
--- a/versionOverview.xlsx
+++ b/versionOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mainnas\webVirtualHost\extranet\dev\GitHub\accounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71835A91-BCE3-43AE-8A20-3D176E9BAFAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F279FA-6739-4038-A5CD-755B5F04ADF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{4C7BC04F-AF9E-4AF1-A85F-469E0888D37E}"/>
+    <workbookView xWindow="10400" yWindow="3580" windowWidth="28800" windowHeight="15460" xr2:uid="{4C7BC04F-AF9E-4AF1-A85F-469E0888D37E}"/>
   </bookViews>
   <sheets>
     <sheet name="Version overview" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="36">
   <si>
     <t>Applikation</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>v2.28.0-beta</t>
+  </si>
+  <si>
+    <t>v1.2.0</t>
+  </si>
+  <si>
+    <t>v1.6.0</t>
   </si>
 </sst>
 </file>
@@ -669,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956BD7F1-73B9-4FB3-85F5-D7C19A133EFA}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,7 +762,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -769,21 +775,21 @@
         <v>27</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="18" t="s">
-        <v>25</v>
+      <c r="F6" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="13" t="s">
-        <v>28</v>
+      <c r="H6" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="9">
-        <v>43613</v>
+        <v>43627</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>23</v>
@@ -804,12 +810,12 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="9">
-        <v>43606</v>
+        <v>43613</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>23</v>
@@ -830,12 +836,12 @@
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="9">
-        <v>43593</v>
+        <v>43606</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>23</v>
@@ -856,12 +862,12 @@
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="9">
-        <v>43583</v>
+        <v>43593</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
-        <v>26</v>
+      <c r="A10" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>23</v>
@@ -873,20 +879,20 @@
         <v>27</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="9">
-        <v>43565</v>
+        <v>43583</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -895,23 +901,25 @@
       <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="18"/>
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="13" t="s">
-        <v>25</v>
+      <c r="H11" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="9">
-        <v>43553</v>
+        <v>43565</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>23</v>
@@ -919,21 +927,23 @@
       <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="7"/>
       <c r="H12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="9">
-        <v>43545</v>
+        <v>43553</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>23</v>
@@ -950,12 +960,12 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="9">
-        <v>43522</v>
+        <v>43545</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>23</v>
@@ -972,12 +982,12 @@
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="9">
-        <v>43521</v>
+        <v>43522</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>23</v>
@@ -989,7 +999,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="13"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="7"/>
@@ -999,7 +1009,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>23</v>
@@ -1011,15 +1021,17 @@
       <c r="E16" s="7"/>
       <c r="F16" s="13"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="I16" s="7"/>
       <c r="J16" s="9">
-        <v>43489</v>
+        <v>43521</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>23</v>
@@ -1034,12 +1046,12 @@
       <c r="H17" s="13"/>
       <c r="I17" s="7"/>
       <c r="J17" s="9">
-        <v>43482</v>
+        <v>43489</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>23</v>
@@ -1054,12 +1066,12 @@
       <c r="H18" s="13"/>
       <c r="I18" s="7"/>
       <c r="J18" s="9">
-        <v>43470</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>23</v>
@@ -1074,12 +1086,12 @@
       <c r="H19" s="13"/>
       <c r="I19" s="7"/>
       <c r="J19" s="9">
-        <v>43469</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>23</v>
@@ -1094,12 +1106,12 @@
       <c r="H20" s="13"/>
       <c r="I20" s="7"/>
       <c r="J20" s="9">
-        <v>43422</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>23</v>
@@ -1114,12 +1126,12 @@
       <c r="H21" s="13"/>
       <c r="I21" s="7"/>
       <c r="J21" s="9">
-        <v>43411</v>
+        <v>43422</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>23</v>
@@ -1139,7 +1151,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>23</v>
@@ -1154,12 +1166,12 @@
       <c r="H23" s="13"/>
       <c r="I23" s="7"/>
       <c r="J23" s="9">
-        <v>43406</v>
+        <v>43411</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>23</v>
@@ -1174,40 +1186,48 @@
       <c r="H24" s="13"/>
       <c r="I24" s="7"/>
       <c r="J24" s="9">
+        <v>43406</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="9">
         <v>43404</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="10">
+      <c r="B26" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="10">
         <v>43401</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
@@ -1232,6 +1252,18 @@
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>